<commit_message>
first commit for the assignment
</commit_message>
<xml_diff>
--- a/src/resources/TestData.xlsx
+++ b/src/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dpworld-my.sharepoint.com/personal/mabassra_cnsonline_net/Documents/Documents/Projects/AsimSwiggy/src/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dulee\eclipse-workspace\DuleekaSwiggy\src\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC10483C515A4B005ADE58F7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{297D8F0A-4B12-4081-83C6-3CAFC7844FCA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407E1E02-031E-4259-A73A-836A91D52D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22950" yWindow="-12765" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>firstname</t>
   </si>
@@ -37,34 +37,40 @@
     <t>postcode</t>
   </si>
   <si>
-    <t>Rashid</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>isita</t>
-  </si>
-  <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Arora</t>
-  </si>
-  <si>
-    <t>Sehgal</t>
-  </si>
-  <si>
-    <t>so3455o</t>
-  </si>
-  <si>
-    <t>Asim</t>
-  </si>
-  <si>
-    <t>Bassra</t>
-  </si>
-  <si>
-    <t>SO15 5RS</t>
+    <t>Duleeka</t>
+  </si>
+  <si>
+    <t>Munasinghe</t>
+  </si>
+  <si>
+    <t>500128S</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>ad3</t>
+  </si>
+  <si>
+    <t>bdge334</t>
+  </si>
+  <si>
+    <t>Kumara</t>
+  </si>
+  <si>
+    <t>Sangakkara</t>
+  </si>
+  <si>
+    <t>Aravinda</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Virath</t>
+  </si>
+  <si>
+    <t>Kholi</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,54 +412,43 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -462,10 +457,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D06F8FE-1C1F-4449-A311-9EDF1BBB245C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7623797D-4C2A-4503-8BC1-9D70B9790055}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>